<commit_message>
Fix responsive layout on mobile devices
</commit_message>
<xml_diff>
--- a/assets/nuget-top-100-package-downloads-20240530.xlsx
+++ b/assets/nuget-top-100-package-downloads-20240530.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github\dylanbeattie\freeasinweekend.org\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F67FFF-069F-4120-B3A4-7EA41468A334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4EBC4A-6005-44C9-B441-0BA7DDC70E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{AD076AC1-60BA-4377-AF8C-7DF2FACC9F51}"/>
+    <workbookView xWindow="34440" yWindow="-690" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AD076AC1-60BA-4377-AF8C-7DF2FACC9F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="#,##0,,&quot;M&quot;"/>
-    <numFmt numFmtId="171" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -690,7 +690,7 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">

</xml_diff>